<commit_message>
Fixed percussion and global transpose PSG (TTFM)
</commit_message>
<xml_diff>
--- a/info/Period table FM - Konami.xlsx
+++ b/info/Period table FM - Konami.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cornelisser\Documents\Dev\TriloTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard.cornelisse\Documents\Dev\TriloTracker\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB44636-67F4-44BF-8BA0-A6FE1D25456A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8EAB10-2CE5-4CB1-9C20-48CAF4D01C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" activeTab="2" xr2:uid="{8DBE4EAE-9AB6-4E70-914F-62B08A727139}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="2" xr2:uid="{8DBE4EAE-9AB6-4E70-914F-62B08A727139}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="63">
   <si>
     <t>Fsam</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Konami value difference:</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Minor Second</t>
   </si>
   <si>
@@ -211,12 +208,30 @@
   <si>
     <t>Default</t>
   </si>
+  <si>
+    <t>ADPCM</t>
+  </si>
+  <si>
+    <t>KHz</t>
+  </si>
+  <si>
+    <t>Conversion Rate</t>
+  </si>
+  <si>
+    <t>Fn = (2^16*72/(3600/R) =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C note = </t>
+  </si>
+  <si>
+    <t>OPL1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,8 +283,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cascadia Mono SemiLight"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -324,6 +345,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -337,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,9 +390,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -388,6 +431,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -400,7 +448,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -698,20 +746,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00566D7-4C98-4E64-90EC-5767F1678F97}">
   <dimension ref="A3:Q34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="11" max="11" width="6.36328125" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" customWidth="1"/>
+    <col min="15" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -719,7 +767,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
@@ -730,7 +778,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D5">
         <f>POWER(2,18)/B3</f>
         <v>5.2428800000000004</v>
@@ -750,12 +798,12 @@
         <v>55.433</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -778,7 +826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -824,7 +872,7 @@
         <v>263.82259728773585</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -870,7 +918,7 @@
         <v>279.65195312499998</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -916,7 +964,7 @@
         <v>297.50207779255317</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -962,7 +1010,7 @@
         <v>314.21567766853934</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1008,7 +1056,7 @@
         <v>332.9189918154762</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1054,7 +1102,7 @@
         <v>353.98981408227849</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1100,7 +1148,7 @@
         <v>377.90804476351349</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1146,7 +1194,7 @@
         <v>399.50279017857144</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1192,7 +1240,7 @@
         <v>423.71508049242425</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1238,7 +1286,7 @@
         <v>443.89198908730157</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1284,7 +1332,7 @@
         <v>473.98636122881356</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1330,12 +1378,12 @@
         <v>499.37848772321428</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:17" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -1352,7 +1400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1395,7 +1443,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1438,7 +1486,7 @@
         <v>A0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1481,7 +1529,7 @@
         <v>AA</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1524,7 +1572,7 @@
         <v>B4</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1567,7 +1615,7 @@
         <v>BE</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1610,7 +1658,7 @@
         <v>CA</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1653,7 +1701,7 @@
         <v>D6</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1696,7 +1744,7 @@
         <v>E2</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -1739,7 +1787,7 @@
         <v>F0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1785,7 +1833,7 @@
         <v>FE</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -1828,7 +1876,7 @@
         <v>10D</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1881,19 +1929,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F012D7-DC4C-472C-8A35-7015F1B53B93}">
   <dimension ref="A1:T44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
-    <col min="10" max="16" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
+    <col min="10" max="16" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H1" t="s">
         <v>29</v>
       </c>
@@ -1901,7 +1949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="H2">
         <v>1.059463</v>
       </c>
@@ -1912,7 +1960,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1963,7 +2011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2027,7 +2075,7 @@
         <v>6.6806288751636353</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2091,7 +2139,7 @@
         <v>6.3056745494308304</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2155,7 +2203,7 @@
         <v>5.9517647614223712</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2219,7 +2267,7 @@
         <v>5.6177183737632843</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2283,7 +2331,7 @@
         <v>5.302420541126291</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2347,7 +2395,7 @@
         <v>5.0048189895506416</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2411,7 +2459,7 @@
         <v>4.7239205045864194</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2475,7 +2523,7 @@
         <v>4.4587876165438711</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2539,7 +2587,7 @@
         <v>4.2085354717851127</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2603,7 +2651,7 @@
         <v>3.9723288796164771</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2667,7 +2715,7 @@
         <v>3.7493795249258137</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2731,7 +2779,7 @@
         <v>3.5389433372621917</v>
       </c>
     </row>
-    <row r="18" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H18" s="5" t="s">
         <v>28</v>
       </c>
@@ -2772,7 +2820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H19">
         <v>1</v>
       </c>
@@ -2817,7 +2865,7 @@
         <v>$0007</v>
       </c>
     </row>
-    <row r="20" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H20">
         <v>2</v>
       </c>
@@ -2826,7 +2874,7 @@
         <v>$06AE</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ref="I20:R30" si="24">_xlfn.CONCAT("$",DEC2HEX(ROUND(J5,0),4))</f>
+        <f t="shared" ref="I20:R28" si="24">_xlfn.CONCAT("$",DEC2HEX(ROUND(J5,0),4))</f>
         <v>$064E</v>
       </c>
       <c r="K20" t="str">
@@ -2862,7 +2910,7 @@
         <v>$0006</v>
       </c>
     </row>
-    <row r="21" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H21">
         <v>3</v>
       </c>
@@ -2907,7 +2955,7 @@
         <v>$0006</v>
       </c>
     </row>
-    <row r="22" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H22">
         <v>4</v>
       </c>
@@ -2952,7 +3000,7 @@
         <v>$0006</v>
       </c>
     </row>
-    <row r="23" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H23">
         <v>5</v>
       </c>
@@ -2997,7 +3045,7 @@
         <v>$0005</v>
       </c>
     </row>
-    <row r="24" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H24">
         <v>6</v>
       </c>
@@ -3042,7 +3090,7 @@
         <v>$0005</v>
       </c>
     </row>
-    <row r="25" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H25">
         <v>7</v>
       </c>
@@ -3087,7 +3135,7 @@
         <v>$0005</v>
       </c>
     </row>
-    <row r="26" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H26">
         <v>8</v>
       </c>
@@ -3132,7 +3180,7 @@
         <v>$0004</v>
       </c>
     </row>
-    <row r="27" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H27">
         <v>9</v>
       </c>
@@ -3177,7 +3225,7 @@
         <v>$0004</v>
       </c>
     </row>
-    <row r="28" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H28">
         <v>10</v>
       </c>
@@ -3222,7 +3270,7 @@
         <v>$0004</v>
       </c>
     </row>
-    <row r="32" spans="8:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H32" s="5" t="s">
         <v>28</v>
       </c>
@@ -3257,7 +3305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H33" t="s">
         <v>6</v>
       </c>
@@ -3302,7 +3350,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H34" t="s">
         <v>7</v>
       </c>
@@ -3347,7 +3395,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H35" t="s">
         <v>8</v>
       </c>
@@ -3392,7 +3440,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H36" t="s">
         <v>9</v>
       </c>
@@ -3437,7 +3485,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H37" t="s">
         <v>10</v>
       </c>
@@ -3482,7 +3530,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="38" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H38" t="s">
         <v>11</v>
       </c>
@@ -3527,7 +3575,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="39" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H39" t="s">
         <v>12</v>
       </c>
@@ -3572,7 +3620,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="40" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H40" t="s">
         <v>13</v>
       </c>
@@ -3617,7 +3665,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="41" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H41" t="s">
         <v>14</v>
       </c>
@@ -3662,7 +3710,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="42" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H42" t="s">
         <v>15</v>
       </c>
@@ -3707,7 +3755,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="43" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H43" t="s">
         <v>16</v>
       </c>
@@ -3752,7 +3800,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="44" spans="8:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="8:18" x14ac:dyDescent="0.35">
       <c r="H44" t="s">
         <v>17</v>
       </c>
@@ -3804,24 +3852,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ED569E-BE75-48B0-8515-4234190F9777}">
-  <dimension ref="A1:AH47"/>
+  <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH30" sqref="AH30"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
+    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="3" max="3" width="2.81640625" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="34" max="34" width="108.44140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="4.6328125" customWidth="1"/>
+    <col min="6" max="6" width="17.36328125" customWidth="1"/>
+    <col min="34" max="34" width="108.453125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
         <v>41</v>
       </c>
@@ -3862,7 +3910,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -3871,7 +3919,7 @@
       </c>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="F3" s="3" t="s">
         <v>27</v>
       </c>
@@ -3912,7 +3960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="61.2" x14ac:dyDescent="1.1000000000000001">
+    <row r="4" spans="1:34" ht="61.5" x14ac:dyDescent="1.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -3923,7 +3971,7 @@
         <v>445</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:N7" si="0">H4/$B$2</f>
+        <f t="shared" ref="G4:N4" si="0">H4/$B$2</f>
         <v>264.60553847467509</v>
       </c>
       <c r="H4">
@@ -3971,7 +4019,7 @@
         <v>499.4926937620001</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -3979,7 +4027,7 @@
         <v>3579545</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="F7" s="5" t="s">
         <v>35</v>
       </c>
@@ -4059,7 +4107,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -4169,12 +4217,12 @@
         <f t="shared" si="13"/>
         <v>$0700</v>
       </c>
-      <c r="AH8" s="10" t="str">
+      <c r="AH8" s="15" t="str">
         <f t="shared" ref="AH8:AH16" si="14">_xlfn.CONCAT("      dw      ",U8,", ",V8,", ",W8,", ",X8,", ",Y8,", ",Z8,", ",AA8,", ",AB8,", ",AC8,", ",AD8,", ",AE8,", ",AF8)</f>
         <v xml:space="preserve">      dw      $0D36, $0C78, $0BC5, $0B1C, $0A7C, $09E6, $0957, $08D1, $0853, $07DB, $076A, $0700</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -4283,12 +4331,12 @@
         <f t="shared" ref="AF9:AF17" si="26">_xlfn.CONCAT("$",DEC2HEX(ROUND(R9,0),4))</f>
         <v>$0380</v>
       </c>
-      <c r="AH9" s="10" t="str">
+      <c r="AH9" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $069B, $063C, $05E3, $058E, $053E, $04F3, $04AC, $0469, $0429, $03ED, $03B5, $0380</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F10">
         <v>3</v>
       </c>
@@ -4391,12 +4439,12 @@
         <f t="shared" si="26"/>
         <v>$01C0</v>
       </c>
-      <c r="AH10" s="10" t="str">
+      <c r="AH10" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $034D, $031E, $02F1, $02C7, $029F, $0279, $0256, $0234, $0215, $01F7, $01DB, $01C0</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F11">
         <v>4</v>
       </c>
@@ -4499,12 +4547,12 @@
         <f t="shared" si="26"/>
         <v>$00E0</v>
       </c>
-      <c r="AH11" s="10" t="str">
+      <c r="AH11" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $01A7, $018F, $0179, $0163, $0150, $013D, $012B, $011A, $010A, $00FB, $00ED, $00E0</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F12">
         <v>5</v>
       </c>
@@ -4607,12 +4655,12 @@
         <f t="shared" si="26"/>
         <v>$0070</v>
       </c>
-      <c r="AH12" s="10" t="str">
+      <c r="AH12" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $00D3, $00C8, $00BC, $00B2, $00A8, $009E, $0095, $008D, $0085, $007E, $0077, $0070</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
         <v>38</v>
       </c>
@@ -4718,12 +4766,12 @@
         <f t="shared" si="26"/>
         <v>$0038</v>
       </c>
-      <c r="AH13" s="10" t="str">
+      <c r="AH13" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $006A, $0064, $005E, $0059, $0054, $004F, $004B, $0047, $0043, $003F, $003B, $0038</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>440</v>
       </c>
@@ -4832,17 +4880,14 @@
         <f t="shared" si="26"/>
         <v>$001C</v>
       </c>
-      <c r="AH14" s="10" t="str">
+      <c r="AH14" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $0035, $0032, $002F, $002C, $002A, $0028, $0025, $0023, $0021, $001F, $001E, $001C</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>448</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
       </c>
       <c r="F15">
         <v>8</v>
@@ -4946,19 +4991,19 @@
         <f t="shared" si="26"/>
         <v>$000E</v>
       </c>
-      <c r="AH15" s="10" t="str">
+      <c r="AH15" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $001A, $0019, $0018, $0016, $0015, $0014, $0013, $0012, $0011, $0010, $000F, $000E</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>445</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
       <c r="F16">
@@ -5063,12 +5108,12 @@
         <f t="shared" si="26"/>
         <v>$0007</v>
       </c>
-      <c r="AH16" s="10" t="str">
+      <c r="AH16" s="15" t="str">
         <f t="shared" si="14"/>
         <v xml:space="preserve">      dw      $000D, $000C, $000C, $000B, $000A, $000A, $0009, $0009, $0008, $0008, $0007, $0007</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>432</v>
       </c>
@@ -5177,12 +5222,15 @@
         <f t="shared" si="26"/>
         <v>$0003</v>
       </c>
-      <c r="AH17" s="10" t="str">
+      <c r="AH17" s="15" t="str">
         <f>_xlfn.CONCAT("      dw      ",U17,", ",V17,", ",W17,", ",X17,", ",Y17,", ",Z17,", ",AA17,", ",AB17,", ",AC17,", ",AD17,", ",AE17,", ",AF17)</f>
         <v xml:space="preserve">      dw      $0007, $0006, $0006, $0006, $0005, $0005, $0005, $0004, $0004, $0004, $0004, $0003</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="AH18" s="15"/>
+    </row>
+    <row r="19" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F19" s="7" t="s">
         <v>34</v>
       </c>
@@ -5261,8 +5309,9 @@
       <c r="AF19" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AH19" s="15"/>
+    </row>
+    <row r="20" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F20">
         <v>1</v>
       </c>
@@ -5365,12 +5414,12 @@
         <f t="shared" si="50"/>
         <v>$0001</v>
       </c>
-      <c r="AH20" s="10" t="str">
+      <c r="AH20" s="15" t="str">
         <f>_xlfn.CONCAT("      dw      ",U20,", ",V20,", ",W20,", ",X20,", ",Y20,", ",Z20,", ",AA20,", ",AB20,", ",AC20,", ",AD20,", ",AE20,", ",AF20)</f>
         <v xml:space="preserve">      dw      $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F21">
         <v>2</v>
       </c>
@@ -5473,12 +5522,12 @@
         <f t="shared" ref="AF21:AF27" si="63">_xlfn.CONCAT("$",DEC2HEX(ROUND(R21,0),4))</f>
         <v>$0380</v>
       </c>
-      <c r="AH21" s="10" t="str">
+      <c r="AH21" s="15" t="str">
         <f t="shared" ref="AH21:AH27" si="64">_xlfn.CONCAT("      dw      ",U21,", ",V21,", ",W21,", ",X21,", ",Y21,", ",Z21,", ",AA21,", ",AB21,", ",AC21,", ",AD21,", ",AE21,", ",AF21)</f>
         <v xml:space="preserve">      dw      $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001, $0001, $03ED, $03B5, $0380</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F22">
         <v>3</v>
       </c>
@@ -5581,14 +5630,14 @@
         <f t="shared" si="63"/>
         <v>$01C0</v>
       </c>
-      <c r="AH22" s="10" t="str">
+      <c r="AH22" s="15" t="str">
         <f t="shared" si="64"/>
         <v xml:space="preserve">      dw      $034D, $031E, $02F1, $02C7, $029F, $0279, $0256, $0234, $0215, $01F7, $01DB, $01C0</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A23" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>4</v>
@@ -5638,7 +5687,7 @@
         <v>237.26477841054069</v>
       </c>
       <c r="R23" s="6">
-        <f t="shared" ref="Q23:R23" si="67">($B$6/R4)/32</f>
+        <f t="shared" ref="R23" si="67">($B$6/R4)/32</f>
         <v>223.9487837299574</v>
       </c>
       <c r="T23">
@@ -5692,20 +5741,20 @@
         <f t="shared" si="63"/>
         <v>$00E0</v>
       </c>
-      <c r="AH23" s="10" t="str">
+      <c r="AH23" s="15" t="str">
         <f t="shared" si="64"/>
         <v xml:space="preserve">      dw      $01A7, $018F, $0179, $0163, $0150, $013D, $012B, $011A, $010A, $00FB, $00ED, $00E0</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>1.0594600000000001</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24">
         <v>5</v>
@@ -5809,14 +5858,14 @@
         <f t="shared" si="63"/>
         <v>$0070</v>
       </c>
-      <c r="AH24" s="10" t="str">
+      <c r="AH24" s="15" t="str">
         <f t="shared" si="64"/>
         <v xml:space="preserve">      dw      $00D3, $00C8, $00BC, $00B2, $00A8, $009E, $0095, $008D, $0085, $007E, $0077, $0070</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25">
         <v>1.12246</v>
@@ -5923,14 +5972,14 @@
         <f t="shared" si="63"/>
         <v>$0038</v>
       </c>
-      <c r="AH25" s="10" t="str">
+      <c r="AH25" s="15" t="str">
         <f t="shared" si="64"/>
         <v xml:space="preserve">      dw      $006A, $0064, $005E, $0059, $0054, $004F, $004B, $0047, $0043, $003F, $003B, $0038</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26">
         <v>1.1892100000000001</v>
@@ -6037,14 +6086,14 @@
         <f t="shared" si="63"/>
         <v>$001C</v>
       </c>
-      <c r="AH26" s="10" t="str">
+      <c r="AH26" s="15" t="str">
         <f t="shared" si="64"/>
         <v xml:space="preserve">      dw      $0035, $0032, $002F, $002C, $002A, $0028, $0025, $0023, $0021, $001F, $001E, $001C</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27">
         <v>1.2599199999999999</v>
@@ -6151,22 +6200,23 @@
         <f t="shared" si="63"/>
         <v>$000E</v>
       </c>
-      <c r="AH27" s="10" t="str">
+      <c r="AH27" s="15" t="str">
         <f t="shared" si="64"/>
         <v xml:space="preserve">      dw      $001A, $0019, $0018, $0016, $0015, $0014, $0013, $0012, $0011, $0010, $000F, $000E</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>1.33483</v>
       </c>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AH28" s="15"/>
+    </row>
+    <row r="29" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29">
         <v>1.41421</v>
@@ -6249,10 +6299,11 @@
       <c r="AF29" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="AH29" s="15"/>
+    </row>
+    <row r="30" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>1.49831</v>
@@ -6260,65 +6311,65 @@
       <c r="F30">
         <v>1</v>
       </c>
-      <c r="T30">
+      <c r="T30" s="16">
         <v>1</v>
       </c>
-      <c r="U30" t="str">
+      <c r="U30" s="16" t="str">
         <f>_xlfn.CONCAT("$",DEC2HEX(G$34+(($T30-1)*512),4))</f>
         <v>$00AD</v>
       </c>
-      <c r="V30" t="str">
-        <f t="shared" ref="V30:AF37" si="81">_xlfn.CONCAT("$",DEC2HEX(H$34+(($T30-1)*512),4))</f>
+      <c r="V30" s="16" t="str">
+        <f t="shared" ref="V30:AF38" si="81">_xlfn.CONCAT("$",DEC2HEX(H$34+(($T30-1)*512),4))</f>
         <v>$00B7</v>
       </c>
-      <c r="W30" t="str">
+      <c r="W30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$00C2</v>
       </c>
-      <c r="X30" t="str">
+      <c r="X30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$00CE</v>
       </c>
-      <c r="Y30" t="str">
+      <c r="Y30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$00DA</v>
       </c>
-      <c r="Z30" t="str">
+      <c r="Z30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$00E7</v>
       </c>
-      <c r="AA30" t="str">
+      <c r="AA30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$00F5</v>
       </c>
-      <c r="AB30" t="str">
+      <c r="AB30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$0103</v>
       </c>
-      <c r="AC30" t="str">
+      <c r="AC30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$0113</v>
       </c>
-      <c r="AD30" t="str">
+      <c r="AD30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$0123</v>
       </c>
-      <c r="AE30" t="str">
+      <c r="AE30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$0134</v>
       </c>
-      <c r="AF30" t="str">
+      <c r="AF30" s="16" t="str">
         <f t="shared" si="81"/>
         <v>$0147</v>
       </c>
-      <c r="AH30" s="10" t="str">
-        <f t="shared" ref="AH30:AH37" si="82">_xlfn.CONCAT("      dw      ",U30,", ",V30,", ",W30,", ",X30,", ",Y30,", ",Z30,", ",AA30,", ",AB30,", ",AC30,", ",AD30,", ",AE30,", ",AF30)</f>
+      <c r="AH30" s="15" t="str">
+        <f t="shared" ref="AH30:AH38" si="82">_xlfn.CONCAT("      dw      ",U30,", ",V30,", ",W30,", ",X30,", ",Y30,", ",Z30,", ",AA30,", ",AB30,", ",AC30,", ",AD30,", ",AE30,", ",AF30)</f>
         <v xml:space="preserve">      dw      $00AD, $00B7, $00C2, $00CE, $00DA, $00E7, $00F5, $0103, $0113, $0123, $0134, $0147</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31">
         <v>1.5873999999999999</v>
@@ -6377,14 +6428,14 @@
         <f t="shared" si="81"/>
         <v>$0347</v>
       </c>
-      <c r="AH31" s="10" t="str">
+      <c r="AH31" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $02AD, $02B7, $02C2, $02CE, $02DA, $02E7, $02F5, $0303, $0313, $0323, $0334, $0347</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32">
         <v>1.6817899999999999</v>
@@ -6396,7 +6447,7 @@
         <v>3</v>
       </c>
       <c r="U32" t="str">
-        <f t="shared" ref="U32:U37" si="83">_xlfn.CONCAT("$",DEC2HEX(G$34+(($T32-1)*512),4))</f>
+        <f t="shared" ref="U32:U38" si="83">_xlfn.CONCAT("$",DEC2HEX(G$34+(($T32-1)*512),4))</f>
         <v>$04AD</v>
       </c>
       <c r="V32" t="str">
@@ -6443,14 +6494,14 @@
         <f t="shared" si="81"/>
         <v>$0547</v>
       </c>
-      <c r="AH32" s="10" t="str">
+      <c r="AH32" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $04AD, $04B7, $04C2, $04CE, $04DA, $04E7, $04F5, $0503, $0513, $0523, $0534, $0547</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33">
         <v>1.7818000000000001</v>
@@ -6509,14 +6560,14 @@
         <f t="shared" si="81"/>
         <v>$0747</v>
       </c>
-      <c r="AH33" s="10" t="str">
+      <c r="AH33" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $06AD, $06B7, $06C2, $06CE, $06DA, $06E7, $06F5, $0703, $0713, $0723, $0734, $0747</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34">
         <v>1.88775</v>
@@ -6623,12 +6674,12 @@
         <f t="shared" si="81"/>
         <v>$0947</v>
       </c>
-      <c r="AH34" s="10" t="str">
+      <c r="AH34" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $08AD, $08B7, $08C2, $08CE, $08DA, $08E7, $08F5, $0903, $0913, $0923, $0934, $0947</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -6689,12 +6740,12 @@
         <f t="shared" si="81"/>
         <v>$0B47</v>
       </c>
-      <c r="AH35" s="10" t="str">
+      <c r="AH35" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $0AAD, $0AB7, $0AC2, $0ACE, $0ADA, $0AE7, $0AF5, $0B03, $0B13, $0B23, $0B34, $0B47</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F36">
         <v>7</v>
       </c>
@@ -6749,12 +6800,12 @@
         <f t="shared" si="81"/>
         <v>$0D47</v>
       </c>
-      <c r="AH36" s="10" t="str">
+      <c r="AH36" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $0CAD, $0CB7, $0CC2, $0CCE, $0CDA, $0CE7, $0CF5, $0D03, $0D13, $0D23, $0D34, $0D47</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" ht="16" x14ac:dyDescent="0.4">
       <c r="F37">
         <v>8</v>
       </c>
@@ -6809,478 +6860,1305 @@
         <f t="shared" si="81"/>
         <v>$0F47</v>
       </c>
-      <c r="AH37" s="10" t="str">
+      <c r="AH37" s="15" t="str">
         <f t="shared" si="82"/>
         <v xml:space="preserve">      dw      $0EAD, $0EB7, $0EC2, $0ECE, $0EDA, $0EE7, $0EF5, $0F03, $0F13, $0F23, $0F34, $0F47</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F38" t="s">
+    <row r="38" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="F38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="T38" s="16">
+        <v>9</v>
+      </c>
+      <c r="U38" s="16" t="str">
+        <f t="shared" si="83"/>
+        <v>$10AD</v>
+      </c>
+      <c r="V38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$10B7</v>
+      </c>
+      <c r="W38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$10C2</v>
+      </c>
+      <c r="X38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$10CE</v>
+      </c>
+      <c r="Y38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$10DA</v>
+      </c>
+      <c r="Z38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$10E7</v>
+      </c>
+      <c r="AA38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$10F5</v>
+      </c>
+      <c r="AB38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$1103</v>
+      </c>
+      <c r="AC38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$1113</v>
+      </c>
+      <c r="AD38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$1123</v>
+      </c>
+      <c r="AE38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$1134</v>
+      </c>
+      <c r="AF38" s="16" t="str">
+        <f t="shared" si="81"/>
+        <v>$1147</v>
+      </c>
+      <c r="AH38" s="15" t="str">
+        <f t="shared" si="82"/>
+        <v xml:space="preserve">      dw      $10AD, $10B7, $10C2, $10CE, $10DA, $10E7, $10F5, $1103, $1113, $1123, $1134, $1147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="AH39" s="15"/>
+    </row>
+    <row r="40" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="B40">
+        <v>16</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T40" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="W40" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="X40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC40" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH40" s="15"/>
+    </row>
+    <row r="41" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41">
+        <f>(2^16*72/(3600/B40))</f>
+        <v>20971.52</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <f>G45/16</f>
+        <v>1310.72</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:R41" si="86">H45/16</f>
+        <v>1388.6554112000001</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="86"/>
+        <v>1471.2248619499524</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="86"/>
+        <v>1558.7038922414968</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="86"/>
+        <v>1651.3844256741763</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="86"/>
+        <v>1749.5757436247629</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="86"/>
+        <v>1853.6055173406914</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="86"/>
+        <v>1963.8209014017691</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="86"/>
+        <v>2080.5896921991184</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="86"/>
+        <v>2204.3015552972784</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="86"/>
+        <v>2335.3693257752548</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="86"/>
+        <v>2474.2303858858513</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="U41" t="str">
+        <f t="shared" ref="U41:U44" si="87">_xlfn.CONCAT("$",DEC2HEX(ROUND(G41,0),4))</f>
+        <v>$051F</v>
+      </c>
+      <c r="V41" t="str">
+        <f t="shared" ref="V41:V46" si="88">_xlfn.CONCAT("$",DEC2HEX(ROUND(H41,0),4))</f>
+        <v>$056D</v>
+      </c>
+      <c r="W41" t="str">
+        <f t="shared" ref="W41:W46" si="89">_xlfn.CONCAT("$",DEC2HEX(ROUND(I41,0),4))</f>
+        <v>$05BF</v>
+      </c>
+      <c r="X41" t="str">
+        <f t="shared" ref="X41:X46" si="90">_xlfn.CONCAT("$",DEC2HEX(ROUND(J41,0),4))</f>
+        <v>$0617</v>
+      </c>
+      <c r="Y41" t="str">
+        <f t="shared" ref="Y41:Y46" si="91">_xlfn.CONCAT("$",DEC2HEX(ROUND(K41,0),4))</f>
+        <v>$0673</v>
+      </c>
+      <c r="Z41" t="str">
+        <f t="shared" ref="Z41:Z46" si="92">_xlfn.CONCAT("$",DEC2HEX(ROUND(L41,0),4))</f>
+        <v>$06D6</v>
+      </c>
+      <c r="AA41" t="str">
+        <f t="shared" ref="AA41:AA46" si="93">_xlfn.CONCAT("$",DEC2HEX(ROUND(M41,0),4))</f>
+        <v>$073E</v>
+      </c>
+      <c r="AB41" t="str">
+        <f t="shared" ref="AB41:AB46" si="94">_xlfn.CONCAT("$",DEC2HEX(ROUND(N41,0),4))</f>
+        <v>$07AC</v>
+      </c>
+      <c r="AC41" t="str">
+        <f t="shared" ref="AC41:AC45" si="95">_xlfn.CONCAT("$",DEC2HEX(ROUND(O41,0),4))</f>
+        <v>$0821</v>
+      </c>
+      <c r="AD41" t="str">
+        <f t="shared" ref="AD41:AD45" si="96">_xlfn.CONCAT("$",DEC2HEX(ROUND(P41,0),4))</f>
+        <v>$089C</v>
+      </c>
+      <c r="AE41" t="str">
+        <f t="shared" ref="AE41:AE45" si="97">_xlfn.CONCAT("$",DEC2HEX(ROUND(Q41,0),4))</f>
+        <v>$091F</v>
+      </c>
+      <c r="AF41" t="str">
+        <f t="shared" ref="AF41:AF45" si="98">_xlfn.CONCAT("$",DEC2HEX(ROUND(R41,0),4))</f>
+        <v>$09AA</v>
+      </c>
+      <c r="AH41" s="15" t="str">
+        <f t="shared" ref="AH41:AH46" si="99">_xlfn.CONCAT("      dw      ",U41,", ",V41,", ",W41,", ",X41,", ",Y41,", ",Z41,", ",AA41,", ",AB41,", ",AC41,", ",AD41,", ",AE41,", ",AF41)</f>
+        <v xml:space="preserve">      dw      $051F, $056D, $05BF, $0617, $0673, $06D6, $073E, $07AC, $0821, $089C, $091F, $09AA</v>
+      </c>
+    </row>
+    <row r="42" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42">
+        <f>$G$4</f>
+        <v>264.60553847467509</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <f>G45/8</f>
+        <v>2621.44</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ref="H42:R42" si="100">H45/8</f>
+        <v>2777.3108224000002</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="100"/>
+        <v>2942.4497238999047</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="100"/>
+        <v>3117.4077844829935</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="100"/>
+        <v>3302.7688513483527</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="100"/>
+        <v>3499.1514872495259</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="100"/>
+        <v>3707.2110346813829</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="100"/>
+        <v>3927.6418028035382</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="100"/>
+        <v>4161.1793843982368</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="100"/>
+        <v>4408.6031105945567</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="100"/>
+        <v>4670.7386515505095</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="100"/>
+        <v>4948.4607717717026</v>
+      </c>
+      <c r="T42">
+        <v>2</v>
+      </c>
+      <c r="U42" t="str">
+        <f t="shared" si="87"/>
+        <v>$0A3D</v>
+      </c>
+      <c r="V42" t="str">
+        <f t="shared" si="88"/>
+        <v>$0AD9</v>
+      </c>
+      <c r="W42" t="str">
+        <f t="shared" si="89"/>
+        <v>$0B7E</v>
+      </c>
+      <c r="X42" t="str">
+        <f t="shared" si="90"/>
+        <v>$0C2D</v>
+      </c>
+      <c r="Y42" t="str">
+        <f t="shared" si="91"/>
+        <v>$0CE7</v>
+      </c>
+      <c r="Z42" t="str">
+        <f t="shared" si="92"/>
+        <v>$0DAB</v>
+      </c>
+      <c r="AA42" t="str">
+        <f t="shared" si="93"/>
+        <v>$0E7B</v>
+      </c>
+      <c r="AB42" t="str">
+        <f t="shared" si="94"/>
+        <v>$0F58</v>
+      </c>
+      <c r="AC42" t="str">
+        <f t="shared" si="95"/>
+        <v>$1041</v>
+      </c>
+      <c r="AD42" t="str">
+        <f t="shared" si="96"/>
+        <v>$1139</v>
+      </c>
+      <c r="AE42" t="str">
+        <f t="shared" si="97"/>
+        <v>$123F</v>
+      </c>
+      <c r="AF42" t="str">
+        <f t="shared" si="98"/>
+        <v>$1354</v>
+      </c>
+      <c r="AH42" s="15" t="str">
+        <f t="shared" si="99"/>
+        <v xml:space="preserve">      dw      $0A3D, $0AD9, $0B7E, $0C2D, $0CE7, $0DAB, $0E7B, $0F58, $1041, $1139, $123F, $1354</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="F43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <f>G45/4</f>
+        <v>5242.88</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ref="H43:R43" si="101">H45/4</f>
+        <v>5554.6216448000005</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="101"/>
+        <v>5884.8994477998094</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="101"/>
+        <v>6234.815568965987</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="101"/>
+        <v>6605.5377026967053</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="101"/>
+        <v>6998.3029744990517</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="101"/>
+        <v>7414.4220693627658</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="101"/>
+        <v>7855.2836056070764</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="101"/>
+        <v>8322.3587687964737</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="101"/>
+        <v>8817.2062211891134</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="101"/>
+        <v>9341.4773031010191</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="101"/>
+        <v>9896.9215435434053</v>
+      </c>
+      <c r="T43">
+        <v>3</v>
+      </c>
+      <c r="U43" t="str">
+        <f t="shared" si="87"/>
+        <v>$147B</v>
+      </c>
+      <c r="V43" t="str">
+        <f t="shared" si="88"/>
+        <v>$15B3</v>
+      </c>
+      <c r="W43" t="str">
+        <f t="shared" si="89"/>
+        <v>$16FD</v>
+      </c>
+      <c r="X43" t="str">
+        <f t="shared" si="90"/>
+        <v>$185B</v>
+      </c>
+      <c r="Y43" t="str">
+        <f t="shared" si="91"/>
+        <v>$19CE</v>
+      </c>
+      <c r="Z43" t="str">
+        <f t="shared" si="92"/>
+        <v>$1B56</v>
+      </c>
+      <c r="AA43" t="str">
+        <f t="shared" si="93"/>
+        <v>$1CF6</v>
+      </c>
+      <c r="AB43" t="str">
+        <f t="shared" si="94"/>
+        <v>$1EAF</v>
+      </c>
+      <c r="AC43" t="str">
+        <f t="shared" si="95"/>
+        <v>$2082</v>
+      </c>
+      <c r="AD43" t="str">
+        <f t="shared" si="96"/>
+        <v>$2271</v>
+      </c>
+      <c r="AE43" t="str">
+        <f t="shared" si="97"/>
+        <v>$247D</v>
+      </c>
+      <c r="AF43" t="str">
+        <f t="shared" si="98"/>
+        <v>$26A9</v>
+      </c>
+      <c r="AH43" s="15" t="str">
+        <f t="shared" si="99"/>
+        <v xml:space="preserve">      dw      $147B, $15B3, $16FD, $185B, $19CE, $1B56, $1CF6, $1EAF, $2082, $2271, $247D, $26A9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44">
+        <f>B41/B42</f>
+        <v>79.255786257879663</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="G44">
+        <f>G45/2</f>
+        <v>10485.76</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ref="H44:R44" si="102">H45/2</f>
+        <v>11109.243289600001</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="102"/>
+        <v>11769.798895599619</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="102"/>
+        <v>12469.631137931974</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="102"/>
+        <v>13211.075405393411</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="102"/>
+        <v>13996.605948998103</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="102"/>
+        <v>14828.844138725532</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="102"/>
+        <v>15710.567211214153</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="102"/>
+        <v>16644.717537592947</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="102"/>
+        <v>17634.412442378227</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="102"/>
+        <v>18682.954606202038</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="102"/>
+        <v>19793.843087086811</v>
+      </c>
+      <c r="T44">
+        <v>4</v>
+      </c>
+      <c r="U44" t="str">
+        <f t="shared" si="87"/>
+        <v>$28F6</v>
+      </c>
+      <c r="V44" t="str">
+        <f t="shared" si="88"/>
+        <v>$2B65</v>
+      </c>
+      <c r="W44" t="str">
+        <f t="shared" si="89"/>
+        <v>$2DFA</v>
+      </c>
+      <c r="X44" t="str">
+        <f t="shared" si="90"/>
+        <v>$30B6</v>
+      </c>
+      <c r="Y44" t="str">
+        <f t="shared" si="91"/>
+        <v>$339B</v>
+      </c>
+      <c r="Z44" t="str">
+        <f t="shared" si="92"/>
+        <v>$36AD</v>
+      </c>
+      <c r="AA44" t="str">
+        <f t="shared" si="93"/>
+        <v>$39ED</v>
+      </c>
+      <c r="AB44" t="str">
+        <f t="shared" si="94"/>
+        <v>$3D5F</v>
+      </c>
+      <c r="AC44" t="str">
+        <f t="shared" si="95"/>
+        <v>$4105</v>
+      </c>
+      <c r="AD44" t="str">
+        <f t="shared" si="96"/>
+        <v>$44E2</v>
+      </c>
+      <c r="AE44" t="str">
+        <f t="shared" si="97"/>
+        <v>$48FB</v>
+      </c>
+      <c r="AF44" t="str">
+        <f t="shared" si="98"/>
+        <v>$4D52</v>
+      </c>
+      <c r="AH44" s="15" t="str">
+        <f t="shared" si="99"/>
+        <v xml:space="preserve">      dw      $28F6, $2B65, $2DFA, $30B6, $339B, $36AD, $39ED, $3D5F, $4105, $44E2, $48FB, $4D52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45" s="13">
+        <f>G4*$B$44</f>
+        <v>20971.52</v>
+      </c>
+      <c r="H45" s="13">
+        <f t="shared" ref="H45:R45" si="103">H4*$B$44</f>
+        <v>22218.486579200002</v>
+      </c>
+      <c r="I45" s="13">
+        <f t="shared" si="103"/>
+        <v>23539.597791199238</v>
+      </c>
+      <c r="J45" s="13">
+        <f t="shared" si="103"/>
+        <v>24939.262275863948</v>
+      </c>
+      <c r="K45" s="13">
+        <f t="shared" si="103"/>
+        <v>26422.150810786821</v>
+      </c>
+      <c r="L45" s="13">
+        <f t="shared" si="103"/>
+        <v>27993.211897996207</v>
+      </c>
+      <c r="M45" s="13">
+        <f t="shared" si="103"/>
+        <v>29657.688277451063</v>
+      </c>
+      <c r="N45" s="13">
+        <f t="shared" si="103"/>
+        <v>31421.134422428306</v>
+      </c>
+      <c r="O45" s="13">
+        <f t="shared" si="103"/>
+        <v>33289.435075185895</v>
+      </c>
+      <c r="P45" s="13">
+        <f t="shared" si="103"/>
+        <v>35268.824884756454</v>
+      </c>
+      <c r="Q45" s="13">
+        <f t="shared" si="103"/>
+        <v>37365.909212404076</v>
+      </c>
+      <c r="R45" s="13">
+        <f t="shared" si="103"/>
+        <v>39587.686174173621</v>
+      </c>
+      <c r="T45">
+        <v>5</v>
+      </c>
+      <c r="U45" t="str">
+        <f t="shared" ref="U45:U46" si="104">_xlfn.CONCAT("$",DEC2HEX(ROUND(G45,0),4))</f>
+        <v>$51EC</v>
+      </c>
+      <c r="V45" t="str">
+        <f t="shared" si="88"/>
+        <v>$56CA</v>
+      </c>
+      <c r="W45" t="str">
+        <f t="shared" si="89"/>
+        <v>$5BF4</v>
+      </c>
+      <c r="X45" t="str">
+        <f t="shared" si="90"/>
+        <v>$616B</v>
+      </c>
+      <c r="Y45" t="str">
+        <f t="shared" si="91"/>
+        <v>$6736</v>
+      </c>
+      <c r="Z45" t="str">
+        <f t="shared" si="92"/>
+        <v>$6D59</v>
+      </c>
+      <c r="AA45" t="str">
+        <f t="shared" si="93"/>
+        <v>$73DA</v>
+      </c>
+      <c r="AB45" t="str">
+        <f t="shared" si="94"/>
+        <v>$7ABD</v>
+      </c>
+      <c r="AC45" t="str">
+        <f t="shared" si="95"/>
+        <v>$8209</v>
+      </c>
+      <c r="AD45" t="str">
+        <f t="shared" si="96"/>
+        <v>$89C5</v>
+      </c>
+      <c r="AE45" t="str">
+        <f t="shared" si="97"/>
+        <v>$91F6</v>
+      </c>
+      <c r="AF45" t="str">
+        <f t="shared" si="98"/>
+        <v>$9AA4</v>
+      </c>
+      <c r="AH45" s="15" t="str">
+        <f t="shared" si="99"/>
+        <v xml:space="preserve">      dw      $51EC, $56CA, $5BF4, $616B, $6736, $6D59, $73DA, $7ABD, $8209, $89C5, $91F6, $9AA4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:34" ht="16" x14ac:dyDescent="0.4">
+      <c r="F46">
+        <v>6</v>
+      </c>
+      <c r="G46">
+        <f>G45*2</f>
+        <v>41943.040000000001</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ref="H46:R46" si="105">H45*2</f>
+        <v>44436.973158400004</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="105"/>
+        <v>47079.195582398475</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="105"/>
+        <v>49878.524551727896</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="105"/>
+        <v>52844.301621573642</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="105"/>
+        <v>55986.423795992414</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="105"/>
+        <v>59315.376554902126</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="105"/>
+        <v>62842.268844856611</v>
+      </c>
+      <c r="O46" s="14">
+        <f t="shared" si="105"/>
+        <v>66578.870150371789</v>
+      </c>
+      <c r="P46" s="14">
+        <f t="shared" si="105"/>
+        <v>70537.649769512907</v>
+      </c>
+      <c r="Q46" s="14">
+        <f t="shared" si="105"/>
+        <v>74731.818424808152</v>
+      </c>
+      <c r="R46" s="14">
+        <f t="shared" si="105"/>
+        <v>79175.372348347242</v>
+      </c>
+      <c r="T46">
+        <v>6</v>
+      </c>
+      <c r="U46" t="str">
+        <f t="shared" si="104"/>
+        <v>$A3D7</v>
+      </c>
+      <c r="V46" t="str">
+        <f t="shared" si="88"/>
+        <v>$AD95</v>
+      </c>
+      <c r="W46" t="str">
+        <f t="shared" si="89"/>
+        <v>$B7E7</v>
+      </c>
+      <c r="X46" t="str">
+        <f t="shared" si="90"/>
+        <v>$C2D7</v>
+      </c>
+      <c r="Y46" t="str">
+        <f t="shared" si="91"/>
+        <v>$CE6C</v>
+      </c>
+      <c r="Z46" t="str">
+        <f t="shared" si="92"/>
+        <v>$DAB2</v>
+      </c>
+      <c r="AA46" t="str">
+        <f t="shared" si="93"/>
+        <v>$E7B3</v>
+      </c>
+      <c r="AB46" t="str">
+        <f t="shared" si="94"/>
+        <v>$F57A</v>
+      </c>
+      <c r="AC46" s="14">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="14">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="14">
+        <v>0</v>
+      </c>
+      <c r="AF46" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="15" t="str">
+        <f t="shared" si="99"/>
+        <v xml:space="preserve">      dw      $A3D7, $AD95, $B7E7, $C2D7, $CE6C, $DAB2, $E7B3, $F57A, 0, 0, 0, 0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F49" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F39" t="s">
+    <row r="50" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F50" t="s">
         <v>42</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G50" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="H50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I50" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J50" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K50" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L39" s="5" t="s">
+      <c r="L50" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M39" s="5" t="s">
+      <c r="M50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N39" s="5" t="s">
+      <c r="N50" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O39" s="5" t="s">
+      <c r="O50" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P39" s="5" t="s">
+      <c r="P50" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q39" s="5" t="s">
+      <c r="Q50" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R39" s="5" t="s">
+      <c r="R50" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F40">
+    <row r="51" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F51">
         <v>1</v>
       </c>
-      <c r="G40">
-        <f>ABS(ROUND(G8,0)-ROUND(G$1,0))</f>
+      <c r="G51">
+        <f t="shared" ref="G51:R51" si="106">ABS(ROUND(G8,0)-ROUND(G$1,0))</f>
         <v>10</v>
       </c>
-      <c r="H40">
-        <f>ABS(ROUND(H8,0)-ROUND(H$1,0))</f>
+      <c r="H51">
+        <f t="shared" si="106"/>
         <v>8</v>
       </c>
-      <c r="I40">
-        <f>ABS(ROUND(I8,0)-ROUND(I$1,0))</f>
+      <c r="I51">
+        <f t="shared" si="106"/>
         <v>5</v>
       </c>
-      <c r="J40">
-        <f>ABS(ROUND(J8,0)-ROUND(J$1,0))</f>
+      <c r="J51">
+        <f t="shared" si="106"/>
         <v>4</v>
       </c>
-      <c r="K40">
-        <f>ABS(ROUND(K8,0)-ROUND(K$1,0))</f>
+      <c r="K51">
+        <f t="shared" si="106"/>
         <v>16</v>
       </c>
-      <c r="L40">
-        <f>ABS(ROUND(L8,0)-ROUND(L$1,0))</f>
+      <c r="L51">
+        <f t="shared" si="106"/>
         <v>6</v>
       </c>
-      <c r="M40">
-        <f>ABS(ROUND(M8,0)-ROUND(M$1,0))</f>
+      <c r="M51">
+        <f t="shared" si="106"/>
         <v>23</v>
       </c>
-      <c r="N40">
-        <f>ABS(ROUND(N8,0)-ROUND(N$1,0))</f>
+      <c r="N51">
+        <f t="shared" si="106"/>
         <v>17</v>
       </c>
-      <c r="O40">
-        <f>ABS(ROUND(O8,0)-ROUND(O$1,0))</f>
+      <c r="O51">
+        <f t="shared" si="106"/>
         <v>19</v>
       </c>
-      <c r="P40">
-        <f>ABS(ROUND(P8,0)-ROUND(P$1,0))</f>
+      <c r="P51">
+        <f t="shared" si="106"/>
         <v>5</v>
       </c>
-      <c r="Q40">
-        <f>ABS(ROUND(Q8,0)-ROUND(Q$1,0))</f>
+      <c r="Q51">
+        <f t="shared" si="106"/>
         <v>10</v>
       </c>
-      <c r="R40">
-        <f>ABS(ROUND(R8,0)-ROUND(R$1,0))</f>
+      <c r="R51">
+        <f t="shared" si="106"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F41">
+    <row r="52" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F52">
         <v>2</v>
       </c>
-      <c r="G41">
-        <f>ABS(ROUND(G9,0)-ROUND((G$1/2),0))</f>
+      <c r="G52">
+        <f t="shared" ref="G52:R52" si="107">ABS(ROUND(G9,0)-ROUND((G$1/2),0))</f>
         <v>5</v>
       </c>
-      <c r="H41">
-        <f>ABS(ROUND(H9,0)-ROUND((H$1/2),0))</f>
+      <c r="H52">
+        <f t="shared" si="107"/>
         <v>4</v>
       </c>
-      <c r="I41">
-        <f>ABS(ROUND(I9,0)-ROUND((I$1/2),0))</f>
+      <c r="I52">
+        <f t="shared" si="107"/>
         <v>3</v>
       </c>
-      <c r="J41">
-        <f>ABS(ROUND(J9,0)-ROUND((J$1/2),0))</f>
+      <c r="J52">
+        <f t="shared" si="107"/>
         <v>2</v>
       </c>
-      <c r="K41">
-        <f>ABS(ROUND(K9,0)-ROUND((K$1/2),0))</f>
+      <c r="K52">
+        <f t="shared" si="107"/>
         <v>8</v>
       </c>
-      <c r="L41">
-        <f>ABS(ROUND(L9,0)-ROUND((L$1/2),0))</f>
+      <c r="L52">
+        <f t="shared" si="107"/>
         <v>3</v>
       </c>
-      <c r="M41">
-        <f>ABS(ROUND(M9,0)-ROUND((M$1/2),0))</f>
+      <c r="M52">
+        <f t="shared" si="107"/>
         <v>12</v>
       </c>
-      <c r="N41">
-        <f>ABS(ROUND(N9,0)-ROUND((N$1/2),0))</f>
+      <c r="N52">
+        <f t="shared" si="107"/>
         <v>9</v>
       </c>
-      <c r="O41">
-        <f>ABS(ROUND(O9,0)-ROUND((O$1/2),0))</f>
+      <c r="O52">
+        <f t="shared" si="107"/>
         <v>9</v>
       </c>
-      <c r="P41">
-        <f>ABS(ROUND(P9,0)-ROUND((P$1/2),0))</f>
+      <c r="P52">
+        <f t="shared" si="107"/>
         <v>3</v>
       </c>
-      <c r="Q41">
-        <f>ABS(ROUND(Q9,0)-ROUND((Q$1/2),0))</f>
+      <c r="Q52">
+        <f t="shared" si="107"/>
         <v>5</v>
       </c>
-      <c r="R41">
-        <f>ABS(ROUND(R9,0)-ROUND((R$1/2),0))</f>
+      <c r="R52">
+        <f t="shared" si="107"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F42">
+    <row r="53" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F53">
         <v>3</v>
       </c>
-      <c r="G42">
-        <f>ABS(ROUND(G10,0)-ROUND((G$1/4),0))</f>
+      <c r="G53">
+        <f t="shared" ref="G53:R53" si="108">ABS(ROUND(G10,0)-ROUND((G$1/4),0))</f>
         <v>3</v>
       </c>
-      <c r="H42">
-        <f>ABS(ROUND(H10,0)-ROUND((H$1/4),0))</f>
+      <c r="H53">
+        <f t="shared" si="108"/>
         <v>2</v>
       </c>
-      <c r="I42">
-        <f>ABS(ROUND(I10,0)-ROUND((I$1/4),0))</f>
+      <c r="I53">
+        <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="J42">
-        <f>ABS(ROUND(J10,0)-ROUND((J$1/4),0))</f>
+      <c r="J53">
+        <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="K42">
-        <f>ABS(ROUND(K10,0)-ROUND((K$1/4),0))</f>
+      <c r="K53">
+        <f t="shared" si="108"/>
         <v>4</v>
       </c>
-      <c r="L42">
-        <f>ABS(ROUND(L10,0)-ROUND((L$1/4),0))</f>
+      <c r="L53">
+        <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="M42">
-        <f>ABS(ROUND(M10,0)-ROUND((M$1/4),0))</f>
+      <c r="M53">
+        <f t="shared" si="108"/>
         <v>6</v>
       </c>
-      <c r="N42">
-        <f>ABS(ROUND(N10,0)-ROUND((N$1/4),0))</f>
+      <c r="N53">
+        <f t="shared" si="108"/>
         <v>4</v>
       </c>
-      <c r="O42">
-        <f>ABS(ROUND(O10,0)-ROUND((O$1/4),0))</f>
+      <c r="O53">
+        <f t="shared" si="108"/>
         <v>5</v>
       </c>
-      <c r="P42">
-        <f>ABS(ROUND(P10,0)-ROUND((P$1/4),0))</f>
+      <c r="P53">
+        <f t="shared" si="108"/>
         <v>1</v>
       </c>
-      <c r="Q42">
-        <f>ABS(ROUND(Q10,0)-ROUND((Q$1/4),0))</f>
+      <c r="Q53">
+        <f t="shared" si="108"/>
         <v>3</v>
       </c>
-      <c r="R42">
-        <f>ABS(ROUND(R10,0)-ROUND((R$1/4),0))</f>
+      <c r="R53">
+        <f t="shared" si="108"/>
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F43">
+    <row r="54" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F54">
         <v>4</v>
       </c>
-      <c r="G43">
-        <f>ABS(ROUND(G11,0)-ROUND((G$1/8),0))</f>
+      <c r="G54">
+        <f t="shared" ref="G54:R54" si="109">ABS(ROUND(G11,0)-ROUND((G$1/8),0))</f>
         <v>1</v>
       </c>
-      <c r="H43">
-        <f>ABS(ROUND(H11,0)-ROUND((H$1/8),0))</f>
+      <c r="H54">
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="I43">
-        <f>ABS(ROUND(I11,0)-ROUND((I$1/8),0))</f>
+      <c r="I54">
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="J43">
-        <f>ABS(ROUND(J11,0)-ROUND((J$1/8),0))</f>
+      <c r="J54">
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="K43">
-        <f>ABS(ROUND(K11,0)-ROUND((K$1/8),0))</f>
+      <c r="K54">
+        <f t="shared" si="109"/>
         <v>2</v>
       </c>
-      <c r="L43">
-        <f>ABS(ROUND(L11,0)-ROUND((L$1/8),0))</f>
+      <c r="L54">
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="M43">
-        <f>ABS(ROUND(M11,0)-ROUND((M$1/8),0))</f>
+      <c r="M54">
+        <f t="shared" si="109"/>
         <v>3</v>
       </c>
-      <c r="N43">
-        <f>ABS(ROUND(N11,0)-ROUND((N$1/8),0))</f>
+      <c r="N54">
+        <f t="shared" si="109"/>
         <v>2</v>
       </c>
-      <c r="O43">
-        <f>ABS(ROUND(O11,0)-ROUND((O$1/8),0))</f>
+      <c r="O54">
+        <f t="shared" si="109"/>
         <v>2</v>
       </c>
-      <c r="P43">
-        <f>ABS(ROUND(P11,0)-ROUND((P$1/8),0))</f>
+      <c r="P54">
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="Q43">
-        <f>ABS(ROUND(Q11,0)-ROUND((Q$1/8),0))</f>
+      <c r="Q54">
+        <f t="shared" si="109"/>
         <v>1</v>
       </c>
-      <c r="R43">
-        <f>ABS(ROUND(R11,0)-ROUND((R$1/8),0))</f>
+      <c r="R54">
+        <f t="shared" si="109"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F44">
+    <row r="55" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F55">
         <v>5</v>
       </c>
-      <c r="G44">
-        <f>ABS(ROUND(G12,0)-ROUND((G$1/16),0))</f>
+      <c r="G55">
+        <f t="shared" ref="G55:R55" si="110">ABS(ROUND(G12,0)-ROUND((G$1/16),0))</f>
         <v>1</v>
       </c>
-      <c r="H44">
-        <f>ABS(ROUND(H12,0)-ROUND((H$1/16),0))</f>
+      <c r="H55">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
-      <c r="I44">
-        <f>ABS(ROUND(I12,0)-ROUND((I$1/16),0))</f>
+      <c r="I55">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
-      <c r="J44">
-        <f>ABS(ROUND(J12,0)-ROUND((J$1/16),0))</f>
+      <c r="J55">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
-      <c r="K44">
-        <f>ABS(ROUND(K12,0)-ROUND((K$1/16),0))</f>
+      <c r="K55">
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="L44">
-        <f>ABS(ROUND(L12,0)-ROUND((L$1/16),0))</f>
+      <c r="L55">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
-      <c r="M44">
-        <f>ABS(ROUND(M12,0)-ROUND((M$1/16),0))</f>
+      <c r="M55">
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="N44">
-        <f>ABS(ROUND(N12,0)-ROUND((N$1/16),0))</f>
+      <c r="N55">
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="O44">
-        <f>ABS(ROUND(O12,0)-ROUND((O$1/16),0))</f>
+      <c r="O55">
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="P44">
-        <f>ABS(ROUND(P12,0)-ROUND((P$1/16),0))</f>
+      <c r="P55">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
-      <c r="Q44">
-        <f>ABS(ROUND(Q12,0)-ROUND((Q$1/16),0))</f>
+      <c r="Q55">
+        <f t="shared" si="110"/>
         <v>1</v>
       </c>
-      <c r="R44">
-        <f>ABS(ROUND(R12,0)-ROUND((R$1/16),0))</f>
+      <c r="R55">
+        <f t="shared" si="110"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F45">
+    <row r="56" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F56">
         <v>6</v>
       </c>
-      <c r="G45">
-        <f>ABS(ROUND(G13,0)-ROUND((G$1/32),0))</f>
+      <c r="G56">
+        <f t="shared" ref="G56:R56" si="111">ABS(ROUND(G13,0)-ROUND((G$1/32),0))</f>
         <v>0</v>
       </c>
-      <c r="H45">
-        <f>ABS(ROUND(H13,0)-ROUND((H$1/32),0))</f>
+      <c r="H56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
-      <c r="I45">
-        <f>ABS(ROUND(I13,0)-ROUND((I$1/32),0))</f>
+      <c r="I56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
-      <c r="J45">
-        <f>ABS(ROUND(J13,0)-ROUND((J$1/32),0))</f>
+      <c r="J56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
-      <c r="K45">
-        <f>ABS(ROUND(K13,0)-ROUND((K$1/32),0))</f>
+      <c r="K56">
+        <f t="shared" si="111"/>
         <v>1</v>
       </c>
-      <c r="L45">
-        <f>ABS(ROUND(L13,0)-ROUND((L$1/32),0))</f>
+      <c r="L56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
-      <c r="M45">
-        <f>ABS(ROUND(M13,0)-ROUND((M$1/32),0))</f>
+      <c r="M56">
+        <f t="shared" si="111"/>
         <v>1</v>
       </c>
-      <c r="N45">
-        <f>ABS(ROUND(N13,0)-ROUND((N$1/32),0))</f>
+      <c r="N56">
+        <f t="shared" si="111"/>
         <v>1</v>
       </c>
-      <c r="O45">
-        <f>ABS(ROUND(O13,0)-ROUND((O$1/32),0))</f>
+      <c r="O56">
+        <f t="shared" si="111"/>
         <v>1</v>
       </c>
-      <c r="P45">
-        <f>ABS(ROUND(P13,0)-ROUND((P$1/32),0))</f>
+      <c r="P56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
-      <c r="Q45">
-        <f>ABS(ROUND(Q13,0)-ROUND((Q$1/32),0))</f>
+      <c r="Q56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
-      <c r="R45">
-        <f>ABS(ROUND(R13,0)-ROUND((R$1/32),0))</f>
+      <c r="R56">
+        <f t="shared" si="111"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F46">
+    <row r="57" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F57">
         <v>7</v>
       </c>
-      <c r="G46">
-        <f>ABS(ROUND(G14,0)-ROUND((G$1/64),0))</f>
+      <c r="G57">
+        <f t="shared" ref="G57:R57" si="112">ABS(ROUND(G14,0)-ROUND((G$1/64),0))</f>
         <v>0</v>
       </c>
-      <c r="H46">
-        <f>ABS(ROUND(H14,0)-ROUND((H$1/64),0))</f>
+      <c r="H57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="I46">
-        <f>ABS(ROUND(I14,0)-ROUND((I$1/64),0))</f>
+      <c r="I57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="J46">
-        <f>ABS(ROUND(J14,0)-ROUND((J$1/64),0))</f>
+      <c r="J57">
+        <f t="shared" si="112"/>
         <v>1</v>
       </c>
-      <c r="K46">
-        <f>ABS(ROUND(K14,0)-ROUND((K$1/64),0))</f>
+      <c r="K57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="L46">
-        <f>ABS(ROUND(L14,0)-ROUND((L$1/64),0))</f>
+      <c r="L57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="M46">
-        <f>ABS(ROUND(M14,0)-ROUND((M$1/64),0))</f>
+      <c r="M57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="N46">
-        <f>ABS(ROUND(N14,0)-ROUND((N$1/64),0))</f>
+      <c r="N57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="O46">
-        <f>ABS(ROUND(O14,0)-ROUND((O$1/64),0))</f>
+      <c r="O57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="P46">
-        <f>ABS(ROUND(P14,0)-ROUND((P$1/64),0))</f>
+      <c r="P57">
+        <f t="shared" si="112"/>
         <v>1</v>
       </c>
-      <c r="Q46">
-        <f>ABS(ROUND(Q14,0)-ROUND((Q$1/64),0))</f>
+      <c r="Q57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
-      <c r="R46">
-        <f>ABS(ROUND(R14,0)-ROUND((R$1/64),0))</f>
+      <c r="R57">
+        <f t="shared" si="112"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
-      <c r="F47">
+    <row r="58" spans="6:18" x14ac:dyDescent="0.35">
+      <c r="F58">
         <v>8</v>
       </c>
-      <c r="G47">
-        <f>ABS(ROUND(G15,0)-ROUND((G$1/128),0))</f>
+      <c r="G58">
+        <f t="shared" ref="G58:R58" si="113">ABS(ROUND(G15,0)-ROUND((G$1/128),0))</f>
         <v>1</v>
       </c>
-      <c r="H47">
-        <f>ABS(ROUND(H15,0)-ROUND((H$1/128),0))</f>
+      <c r="H58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="I47">
-        <f>ABS(ROUND(I15,0)-ROUND((I$1/128),0))</f>
+      <c r="I58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="J47">
-        <f>ABS(ROUND(J15,0)-ROUND((J$1/128),0))</f>
+      <c r="J58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="K47">
-        <f>ABS(ROUND(K15,0)-ROUND((K$1/128),0))</f>
+      <c r="K58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="L47">
-        <f>ABS(ROUND(L15,0)-ROUND((L$1/128),0))</f>
+      <c r="L58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="M47">
-        <f>ABS(ROUND(M15,0)-ROUND((M$1/128),0))</f>
+      <c r="M58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="N47">
-        <f>ABS(ROUND(N15,0)-ROUND((N$1/128),0))</f>
+      <c r="N58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="O47">
-        <f>ABS(ROUND(O15,0)-ROUND((O$1/128),0))</f>
+      <c r="O58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="P47">
-        <f>ABS(ROUND(P15,0)-ROUND((P$1/128),0))</f>
+      <c r="P58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="Q47">
-        <f>ABS(ROUND(Q15,0)-ROUND((Q$1/128),0))</f>
+      <c r="Q58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
-      <c r="R47">
-        <f>ABS(ROUND(R15,0)-ROUND((R$1/128),0))</f>
+      <c r="R58">
+        <f t="shared" si="113"/>
         <v>0</v>
       </c>
     </row>
@@ -7290,15 +8168,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U20:AF22">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
-      <formula>"$0001"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40:R47">
+  <conditionalFormatting sqref="G51:R58">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -7318,7 +8188,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <conditionalFormatting sqref="U20:AF22">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"$0001"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4" xr:uid="{0E864412-12D8-4B93-8518-B319BC23E620}">
       <formula1>$A$14:$A$18</formula1>
     </dataValidation>

</xml_diff>